<commit_message>
couleurs + direction du vent
</commit_message>
<xml_diff>
--- a/infos_filtres.xlsx
+++ b/infos_filtres.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="14000" yWindow="0" windowWidth="11600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
   <si>
     <t>Couleur</t>
   </si>
@@ -103,6 +103,51 @@
   </si>
   <si>
     <t>XX</t>
+  </si>
+  <si>
+    <t>Direction du vent</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>MTD</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -244,8 +289,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -362,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="109">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -412,6 +467,11 @@
     <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -461,6 +521,11 @@
     <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -790,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -805,7 +870,7 @@
     <col min="11" max="11" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -815,135 +880,168 @@
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>180</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>216</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>217</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>218</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" t="s">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" t="s">
+      <c r="L5" s="12"/>
+      <c r="M5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>219</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6">
         <v>6</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>268</v>
       </c>
@@ -953,22 +1051,22 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>269</v>
       </c>
@@ -978,78 +1076,120 @@
       <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>8</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>359</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
         <v>9</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>360</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>361</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>362</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>363</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>364</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>365</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>366</v>
       </c>
@@ -1057,63 +1197,111 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>367</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>370</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>371</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>372</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>373</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>374</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>375</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>433</v>
       </c>
@@ -1121,196 +1309,340 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>528</v>
       </c>
       <c r="B25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>531</v>
       </c>
       <c r="B26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>533</v>
       </c>
       <c r="B27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>534</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>535</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>537</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>538</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>539</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>540</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>541</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>544</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>555</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>557</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>560</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>564</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>565</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>566</v>
       </c>
       <c r="B41">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>567</v>
       </c>
       <c r="B42">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>568</v>
       </c>
       <c r="B43">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>569</v>
       </c>
       <c r="B44">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>570</v>
       </c>
       <c r="B45">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>575</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>590</v>
       </c>
       <c r="B47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>603</v>
       </c>
       <c r="B48">
         <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1320,6 +1652,12 @@
       <c r="B49">
         <v>6</v>
       </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
@@ -1328,6 +1666,12 @@
       <c r="B50">
         <v>2</v>
       </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
       <c r="H50" s="4" t="s">
         <v>15</v>
       </c>
@@ -1342,6 +1686,12 @@
       <c r="B51">
         <v>4</v>
       </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
       <c r="G51">
         <v>2</v>
       </c>
@@ -1359,6 +1709,12 @@
       <c r="B52">
         <v>3</v>
       </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
       <c r="G52">
         <v>3</v>
       </c>
@@ -1374,6 +1730,12 @@
       <c r="B53">
         <v>4</v>
       </c>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
       <c r="G53">
         <v>4</v>
       </c>
@@ -1388,6 +1750,12 @@
       </c>
       <c r="B54">
         <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s">
+        <v>31</v>
       </c>
       <c r="G54">
         <v>5</v>

</xml_diff>

<commit_message>
rose des vents pimpée
</commit_message>
<xml_diff>
--- a/infos_filtres.xlsx
+++ b/infos_filtres.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="46">
   <si>
     <t>Couleur</t>
   </si>
@@ -129,9 +129,6 @@
     <t>MTD</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
@@ -145,6 +142,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>NNE</t>
+  </si>
+  <si>
+    <t>ENE</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>ESE</t>
+  </si>
+  <si>
+    <t>NNO</t>
   </si>
 </sst>
 </file>
@@ -854,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -907,7 +919,7 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -937,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -965,7 +977,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -993,7 +1005,7 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1021,7 +1033,7 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -1048,6 +1060,9 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
       <c r="G7">
         <v>7</v>
       </c>
@@ -1073,6 +1088,9 @@
       <c r="C8" t="s">
         <v>28</v>
       </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
       <c r="G8">
         <v>8</v>
       </c>
@@ -1092,7 +1110,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>9</v>
@@ -1141,7 +1159,7 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1155,7 +1173,7 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1169,7 +1187,7 @@
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1183,7 +1201,7 @@
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1197,7 +1215,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1208,7 +1226,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
@@ -1225,7 +1243,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1236,10 +1254,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1267,7 +1285,7 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1281,7 +1299,7 @@
         <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1295,7 +1313,7 @@
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1323,7 +1341,7 @@
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1334,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
         <v>30</v>
@@ -1348,10 +1366,10 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1365,7 +1383,7 @@
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1379,7 +1397,7 @@
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1393,7 +1411,7 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1407,7 +1425,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1421,7 +1439,7 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1435,7 +1453,7 @@
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1449,7 +1467,7 @@
         <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1463,7 +1481,7 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1474,10 +1492,10 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1485,10 +1503,10 @@
         <v>415</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1513,10 +1531,10 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1530,7 +1548,7 @@
         <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1544,7 +1562,7 @@
         <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1558,7 +1576,7 @@
         <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1572,7 +1590,7 @@
         <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1586,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1600,7 +1618,7 @@
         <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1611,7 +1629,7 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
         <v>41</v>
@@ -1625,7 +1643,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
         <v>30</v>
@@ -1639,10 +1657,10 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1656,7 +1674,7 @@
         <v>34</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1670,7 +1688,7 @@
         <v>28</v>
       </c>
       <c r="D50" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1684,7 +1702,7 @@
         <v>31</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1709,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D53" t="s">
         <v>30</v>
@@ -1740,7 +1758,7 @@
         <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1754,7 +1772,7 @@
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1768,7 +1786,7 @@
         <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1824,7 +1842,7 @@
         <v>32</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1838,7 +1856,7 @@
         <v>31</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -1849,7 +1867,7 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
         <v>30</v>
@@ -1866,7 +1884,7 @@
         <v>28</v>
       </c>
       <c r="D64" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>15</v>
@@ -1930,7 +1948,7 @@
         <v>31</v>
       </c>
       <c r="D67" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G67">
         <v>4</v>
@@ -1951,7 +1969,7 @@
         <v>31</v>
       </c>
       <c r="D68" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G68">
         <v>5</v>
@@ -2014,7 +2032,7 @@
         <v>28</v>
       </c>
       <c r="D71" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G71">
         <v>8</v>
@@ -2035,7 +2053,7 @@
         <v>32</v>
       </c>
       <c r="D72" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G72">
         <v>9</v>
@@ -2056,7 +2074,7 @@
         <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2070,7 +2088,7 @@
         <v>34</v>
       </c>
       <c r="D74" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2112,7 +2130,7 @@
         <v>31</v>
       </c>
       <c r="D77" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2126,7 +2144,7 @@
         <v>32</v>
       </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>